<commit_message>
Added Japanese localization of more check.
</commit_message>
<xml_diff>
--- a/Config/JP/Checklist.xlsx
+++ b/Config/JP/Checklist.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C71E11-DF4E-4F54-AEEF-76561904CCDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D78E6-00D3-41FD-82D8-E230C388257E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ワークフロー" sheetId="2" r:id="rId1"/>
@@ -23,39 +23,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
   <si>
-    <t>Explanation</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Suggestion</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Check Filename</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Argument</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Issue</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>(^(dt_)*([A-Z][a-z0-9]*)+$)</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>(^(in_|out_|io_)(dt_)*([A-Z][a-z0-9]*)+)</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Run</t>
-  </si>
-  <si>
-    <t>Issue</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>最上位階層のアクティビティ（基本的にFlowchartやSequence）には、ワークフローの目的・概要を簡潔に注釈することを推奨します。これにより、開発者はワークフローの目的・インプット・アウトプット・前提条件を素早く把握することができます。</t>
@@ -101,7 +74,7 @@
     <rPh sb="110" eb="112">
       <t>ハアク</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>最上位階層のアクティビティには、ワークフローの概要を注釈することを推奨します。</t>
@@ -120,7 +93,7 @@
     <rPh sb="33" eb="35">
       <t>スイショウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>注釈の欠落</t>
@@ -130,14 +103,14 @@
     <rPh sb="3" eb="5">
       <t>ケツラク</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>スクリーンショットの欠落</t>
     <rPh sb="10" eb="12">
       <t>ケツラク</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>スクリーンショットは、アクティビティがどの要素に対してどういった処理を実行するか確認するのに有効です。各スクリーンショットは、プロジェクト内の「.screenshots」フォルダに、保存されている必要があります。</t>
@@ -171,7 +144,7 @@
     <rPh sb="98" eb="100">
       <t>ヒツヨウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>有効なスクリーンショットを参照してください。</t>
@@ -181,7 +154,7 @@
     <rPh sb="13" eb="15">
       <t>サンショウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>注釈の無い待機（Delay）</t>
@@ -194,7 +167,7 @@
     <rPh sb="5" eb="7">
       <t>タイキ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>待機（Delay）は、必要以上にロボットのパフォーマンスを低下させることがあるので、その使用は最小限にすることを推奨しています。UI同期の方法は、待機（Delay）以外の方法を含めて、こちらのページで紹介されています。https://studio.uipath.com/lang-ja/docs/ui-automation#section-ui-synchronization</t>
@@ -240,7 +213,7 @@
     <rPh sb="100" eb="102">
       <t>ショウカイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>アプリケーションの状態変化を待つ方法として、待機（Delay）以外を検討してください。待機（Delay）が絶対に必要な状況の場合は、その理由を注釈に記載してください。</t>
@@ -280,14 +253,14 @@
     <rPh sb="74" eb="76">
       <t>キサイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>空のキャッチ（Catch）ブロック</t>
     <rPh sb="0" eb="1">
       <t>カラ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>例外のキャッチは、ただエラーメッセージを回避するためでなく、目的を持って行われるべきです。そのため、トライキャッチ（Try Catch）のキャッチブロックには、ログメッセージの出力を推奨しています。エラー処理に関する情報はこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/project-organization#section-error-handling</t>
@@ -324,7 +297,7 @@
     <rPh sb="119" eb="121">
       <t>ショウカイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>例外をキャッチした際に対応することがない場合でも、少なくともログメッセージを出力することを推奨します。</t>
@@ -349,7 +322,7 @@
     <rPh sb="45" eb="47">
       <t>スイショウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>命名規則違反（変数）</t>
@@ -365,7 +338,7 @@
     <rPh sb="7" eb="9">
       <t>ヘンスウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>命名規則違反（引数）</t>
@@ -381,7 +354,7 @@
     <rPh sb="7" eb="9">
       <t>ヒキスウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>変数の命名は、ワークフローの保守性を維持するため、指定された命名規則を守る必要があります。こちらのチェックは、正規表現を引数として受け取り、それを守っているかどうかを確認する機能となります。命名規則に関してはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/workflow-design#section-naming-conventions</t>
@@ -451,14 +424,14 @@
     <rPh sb="112" eb="114">
       <t>ショウカイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>引数の命名は、ワークフローの保守性を維持するため、指定された命名規則を守る必要があります。こちらのチェックは、正規表現を引数として受け取り、それを守っているかどうかを確認する機能となります。命名規則に関してはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/workflow-design#section-naming-conventions</t>
     <rPh sb="0" eb="2">
       <t>ヒキスウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>変数名は命名規則に従って命名してください。</t>
@@ -477,14 +450,14 @@
     <rPh sb="12" eb="14">
       <t>メイメイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>引数名は命名規則に従って命名してください。</t>
     <rPh sb="0" eb="2">
       <t>ヒキスウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>idx属性値が大きいので、セレクターにidx属性以外の属性を追加することを検討してください。</t>
@@ -509,7 +482,7 @@
     <rPh sb="37" eb="39">
       <t>ケントウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>セレクターのidx属性は、同じセレクターで取得できる要素を、要素の順序に基づいて判別するために使われます。この順序は、画面の要素が変わると、それに伴って変わってしまうことがあります。誤った要素を選択することを避けるため、idx属性の値はできるだけ小さい値となるようにセレクターを構築することを推奨します。こちらのチェックは、引数としてidx属性の閾値を受け取り、その値より大きいか確認しています。セレクターについてはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/ui-automation#section-selectors</t>
@@ -615,7 +588,7 @@
     <rPh sb="216" eb="218">
       <t>ショウカイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>セレクターのidx属性値が過大</t>
@@ -628,14 +601,14 @@
     <rPh sb="13" eb="15">
       <t>カダイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>不必要なシーケンス（Sequence）やフローチャート（Flowchart）</t>
     <rPh sb="0" eb="3">
       <t>フヒツヨウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ワークフロー上において、シーケンスは特定の目的を果たすために使用されます。そのため、空のシーケンスは、ワークフローの可読性を低めるだけなので、使用されるべきではありません。また、内部にアクティビティを１つしか含まないシーケンスやフローチャートは、基本的に削除してもワークフローの動作に影響を及ぼしません。 シーケンスの削除には、 コンテキストメニューのシーケンスを削除（Remove Sequence）オプションを使用することができます。 (https://studio.uipath.com/lang-ja/docs/the-user-interface#section-the-context-menu).</t>
@@ -696,7 +669,7 @@
     <rPh sb="207" eb="209">
       <t>シヨウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>実行されないアクティビティの削除を検討してください。</t>
@@ -709,7 +682,7 @@
     <rPh sb="17" eb="19">
       <t>ケントウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>空の、もしくは、内部にアクティビティを1つしか含まないシーケンス・フローチャートの削除を検討してください。</t>
@@ -728,7 +701,7 @@
     <rPh sb="44" eb="46">
       <t>ケントウ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>ワークフロー上には、実行時に必要なアクティビティのみ配置されるべきです。コメントアウトされたアクティビティや、フローチャート上でどのノードにも接続されていないアクティビティは削除することを推奨します。コメントアウトしたアクティビティを保持することが必要な場合は、その理由を注釈してください。</t>
@@ -774,7 +747,7 @@
     <rPh sb="136" eb="138">
       <t>チュウシャク</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>プロジェクト設定ファイル (project.json) の欠落</t>
@@ -784,7 +757,7 @@
     <rPh sb="29" eb="31">
       <t>ケツラク</t>
     </rPh>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="4"/>
   </si>
   <si>
     <t>project.jsonファイルには、プロジェクトに関する重要な情報が含まれており、UiPathStudioでプロジェクトを読み込む際に使用されています。 project.jsonファイルについてはこちらのページで紹介されています。 https://studio.uipath.com/lang-ja/docs/about-the-projectjson-file</t>
@@ -815,180 +788,380 @@
     <rPh sb="107" eb="109">
       <t>ショウカイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>project.jsonファイルを作成もしくはインポートしてください。</t>
     <rPh sb="17" eb="19">
       <t>サクセイ</t>
     </rPh>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented default click</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since they do not depend on the mouse driver, the properties SimulateClick and SendWindowMessages provide a faster and more robust way to perform clicks, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateClick or SendWindowMessages if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented default type</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Since they do not depend on the keyboard driver, the properties SimulateType and SendWindowMessages provide a faster and more robust way to perform typing actions, so they should be used whenever possible. Alternatively, add an annotation in case the control does not support such properties. For more about input methods, refer to https://studio.uipath.com/docs/ui-automation#section-input-methods</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Use SimulateType or SendWindowMessages if the target control supports it.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Undocumented unreachable activities</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Action</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Fix</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Double check</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\ProjectJsonConfigurationFile.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\MissingWorkflowAnnotation.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\MissingScreenshot.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\UndocumentedDelay.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\EmptyCatchBlock.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\VariableNamingConvention.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\ArgumentNamingConvention.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\UndocumentedDefaultClick.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\UnnecessarySequenceOrFlowchart.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\UndocumentedUnreachableActivities.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\LargeIdxInSelector.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\UndocumentedDefaultType.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Yes</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Yes</t>
   </si>
   <si>
-    <t>Variable scope is not the innermost</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variables should be defined in the innermost scope possible to improve the workflow's organization and avoid unintended usage in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Restrict the scope of the variable.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\VariableMinimumScope\VariableMinimumScope.xaml</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\VariableOverridesVariable.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for a variable and an argument have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Although it is technically possible for two variables to have the same name, it can lead to confusion about which is used and make the process of debugging more difficult.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables, even if they are in different scopes.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Define unique names for variables and arguments.</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\VariableOverridesArgument.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable overrides argument</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Variable overrides variable</t>
-    <phoneticPr fontId="6"/>
+    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>注釈の無いデフォルトのクリック（Click）</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>クリックをシミュレート（SimulateClick）やウィンドウメッセージを送信（SendWindowMessages）は、マウスドライバーを使用しないため、より高速で安定したクリックを実行することができます。そのため、これらオプションを使用して正常に動作する場合は、常に使用することを推奨します。両オプションとも正常に動かない場合は、その旨を注釈に記入しデフォルトのクリックを使用してください。両オプションについてはこちらで紹介されています。 https://studio.uipath.com/lang-ja/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>正常に動作しない場合を除き、クリックをシミュレート（SimulateClick）もしくはウィンドウメッセージを送信（SendWindowMessages）を使用することを推奨します。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>注釈の無いデフォルトの入力（Type）</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>入力をシミュレート（SimulateType）ウィンドウメッセージを送信（SendWindowMessages）は、キーボードドライバーを使用しないため、より高速で安定した入力を実行することができます。そのため、これらのオプションを使用して正常に動作する場合は、常に使用することを推奨します。 両オプションとも正常に動かない場合は、その旨を注釈に記入しデフォルトの入力を使用してください。両オプションについてはこちらで紹介されています。 https://studio.uipath.com/lang-ja/docs/ui-automation#section-input-methods</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>正常に動作しない場合を除き、入力をシミュレート（SimulateType）もしくはウィンドウメッセージを送信（SendWindowMessages）を使用することを推奨します。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>注釈の無い実行されないアクティビティ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>必要最小限でない変数のスコープ</t>
+    <rPh sb="0" eb="2">
+      <t>ヒツヨウ</t>
+    </rPh>
+    <rPh sb="2" eb="5">
+      <t>サイショウゲン</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヘンスウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数のスコープは必要最小限の範囲にするべきです。ワークフローの構成の改善や、変数が想定外の利用をされるのを防ぐことにつながります。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="8" eb="13">
+      <t>ヒツヨウサイショウゲン</t>
+    </rPh>
+    <rPh sb="14" eb="16">
+      <t>ハンイ</t>
+    </rPh>
+    <rPh sb="31" eb="33">
+      <t>コウセイ</t>
+    </rPh>
+    <rPh sb="34" eb="36">
+      <t>カイゼン</t>
+    </rPh>
+    <rPh sb="38" eb="40">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="41" eb="43">
+      <t>ソウテイ</t>
+    </rPh>
+    <rPh sb="43" eb="44">
+      <t>ガイ</t>
+    </rPh>
+    <rPh sb="45" eb="47">
+      <t>リヨウ</t>
+    </rPh>
+    <rPh sb="53" eb="54">
+      <t>フセ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数のスコープを最小限にしてください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="8" eb="11">
+      <t>サイショウゲン</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>複数の変数が同じ変数名を持つことは技術的に可能ですが、避けるべきです。どちらの変数が使われているかわからなくなり、デバッグが煩雑になってしまいます。</t>
+    <rPh sb="0" eb="2">
+      <t>フクスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="10" eb="11">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="12" eb="13">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="17" eb="20">
+      <t>ギジュツテキ</t>
+    </rPh>
+    <rPh sb="21" eb="23">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="39" eb="41">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="42" eb="43">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="62" eb="64">
+      <t>ハンザツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数名の重複</t>
+    <rPh sb="0" eb="3">
+      <t>ヘンスウメイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>チョウフク</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数名と引数名の重複</t>
+    <rPh sb="0" eb="3">
+      <t>ヘンスウメイ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>メイ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>チョウフク</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数と引数が同じ名前を持つことは技術的に可能ですが、避けるべきです。どちらが使われているかわからなくなり、デバッグが煩雑になってしまいます。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="6" eb="7">
+      <t>オナ</t>
+    </rPh>
+    <rPh sb="8" eb="10">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>モ</t>
+    </rPh>
+    <rPh sb="16" eb="19">
+      <t>ギジュツテキ</t>
+    </rPh>
+    <rPh sb="20" eb="22">
+      <t>カノウ</t>
+    </rPh>
+    <rPh sb="38" eb="39">
+      <t>ツカ</t>
+    </rPh>
+    <rPh sb="58" eb="60">
+      <t>ハンザツ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数と引数には重複しない名前を定義してください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>ヒキスウ</t>
+    </rPh>
+    <rPh sb="7" eb="9">
+      <t>チョウフク</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="15" eb="17">
+      <t>テイギ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>変数には重複しない名前を定義してください。異なるスコープであっても変数名の重複を避けてください。</t>
+    <rPh sb="0" eb="2">
+      <t>ヘンスウ</t>
+    </rPh>
+    <rPh sb="4" eb="6">
+      <t>チョウフク</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>ナマエ</t>
+    </rPh>
+    <rPh sb="12" eb="14">
+      <t>テイギ</t>
+    </rPh>
+    <rPh sb="33" eb="36">
+      <t>ヘンスウメイ</t>
+    </rPh>
+    <rPh sb="37" eb="39">
+      <t>チョウフク</t>
+    </rPh>
+    <rPh sb="40" eb="41">
+      <t>サ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>実行</t>
+    <rPh sb="0" eb="2">
+      <t>ジッコウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>事象</t>
+    <rPh sb="0" eb="2">
+      <t>ジショウ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>チェックファイル</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>引数</t>
+    <rPh sb="0" eb="2">
+      <t>ヒキスウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>説明</t>
+    <rPh sb="0" eb="2">
+      <t>セツメイ</t>
+    </rPh>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>メッセージ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>修正</t>
+    <rPh sb="0" eb="2">
+      <t>シュウセイ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>確認</t>
+    <rPh sb="0" eb="2">
+      <t>カクニン</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>確認</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>対応</t>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Yu Gothic"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Yu Gothic"/>
-      <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1090,20 +1263,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1114,19 +1281,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1426,330 +1593,330 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="90">
+      <c r="A2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="72">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="10" t="s">
+    </row>
+    <row r="4" spans="1:7" s="3" customFormat="1" ht="108">
+      <c r="A4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="3" customFormat="1" ht="126">
+      <c r="A5" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="3" customFormat="1" ht="126">
+      <c r="A6" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" ht="126">
+      <c r="A7" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="180">
+      <c r="A8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="3" customFormat="1" ht="180">
+      <c r="A9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" ht="180">
+      <c r="A10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="4">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="90">
-      <c r="A2" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="72">
-      <c r="A3" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="108">
-      <c r="A4" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="126">
-      <c r="A5" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="4" t="s">
+      <c r="E10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="5" customFormat="1" ht="126">
-      <c r="A6" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" s="5" customFormat="1" ht="126">
-      <c r="A7" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="5" customFormat="1" ht="144">
-      <c r="A8" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="5" customFormat="1" ht="144">
-      <c r="A9" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="5" customFormat="1" ht="180">
-      <c r="A10" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="180">
-      <c r="A11" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>33</v>
+      <c r="A11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="108">
-      <c r="A12" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>32</v>
+      <c r="B12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="54">
-      <c r="A13" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>64</v>
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="54">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="54">
+      <c r="A15" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="72">
-      <c r="A15" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="4" t="s">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C15" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>70</v>
+      <c r="F15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5"/>
+  <phoneticPr fontId="4"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{D6548621-3B12-46F1-AA74-303D6C198CDC}">
       <formula1>"Yes, No"</formula1>
@@ -1764,9 +1931,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
   <cols>
@@ -1779,51 +1944,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
-      <c r="A1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>8</v>
+      <c r="A1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="5" customFormat="1" ht="108">
-      <c r="A2" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
+    <row r="2" spans="1:7" s="3" customFormat="1" ht="108">
+      <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="5"/>
+  <phoneticPr fontId="4"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{17BA02FB-83C0-4B44-8ABF-D63FDA63E81F}">
       <formula1>"Yes, No"</formula1>

</xml_diff>

<commit_message>
Added dropdown menu for action to be taken regarding a problem (Fix, Double check).
</commit_message>
<xml_diff>
--- a/Config/JP/Checklist.xlsx
+++ b/Config/JP/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401D78E6-00D3-41FD-82D8-E230C388257E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB337A47-2ABB-4B7E-A794-DD7A7CD3B14F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="76">
   <si>
     <t>(^(dt_)*([A-Z][a-z0-9]*)+$)</t>
     <phoneticPr fontId="4"/>
@@ -1141,15 +1141,17 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
+    <t>対応</t>
+    <rPh sb="0" eb="2">
+      <t>タイオウ</t>
+    </rPh>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
     <t>確認</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>対応</t>
-    <rPh sb="0" eb="2">
-      <t>タイオウ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>修正</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1581,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58203125" defaultRowHeight="18"/>
   <cols>
@@ -1606,7 +1610,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>69</v>
@@ -1757,7 +1761,7 @@
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>50</v>
@@ -1778,7 +1782,7 @@
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>53</v>
@@ -1801,7 +1805,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>21</v>
@@ -1822,7 +1826,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
@@ -1843,7 +1847,7 @@
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
@@ -1864,7 +1868,7 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>57</v>
@@ -1885,7 +1889,7 @@
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>59</v>
@@ -1906,7 +1910,7 @@
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>62</v>
@@ -1917,9 +1921,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4"/>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A15" xr:uid="{D6548621-3B12-46F1-AA74-303D6C198CDC}">
       <formula1>"Yes, No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E15" xr:uid="{6CC92C5C-67A3-465A-9410-BA22611AEE61}">
+      <formula1>"修正, 確認"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1957,7 +1964,7 @@
         <v>68</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Changed Project Checks so that it's possible for one check to have multiple issues in the report.
</commit_message>
<xml_diff>
--- a/Config/JP/Checklist.xlsx
+++ b/Config/JP/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02BADCA2-FEE5-4975-B42F-DCA9995681A3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889FC2AE-BC57-453B-997B-1B3EA1324F2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ワークフロー" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="103">
   <si>
     <t>(^(dt_)*([A-Z][a-z0-9]*)+$)</t>
     <phoneticPr fontId="5"/>
@@ -862,9 +862,6 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>No</t>
-  </si>
-  <si>
     <t>注釈の無いデフォルトのクリック（Click）</t>
     <phoneticPr fontId="6"/>
   </si>
@@ -1715,10 +1712,6 @@
   </si>
   <si>
     <t>Checks\RepeatedActivityName.xaml</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Yes</t>
     <phoneticPr fontId="5"/>
   </si>
 </sst>
@@ -2170,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
@@ -2187,30 +2180,30 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="93.75">
       <c r="A2" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
@@ -2220,7 +2213,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -2231,7 +2224,7 @@
     </row>
     <row r="3" spans="1:7" s="3" customFormat="1" ht="93.75">
       <c r="A3" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -2241,7 +2234,7 @@
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>6</v>
@@ -2252,7 +2245,7 @@
     </row>
     <row r="4" spans="1:7" s="3" customFormat="1" ht="112.5">
       <c r="A4" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>8</v>
@@ -2262,7 +2255,7 @@
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>9</v>
@@ -2273,7 +2266,7 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="131.25">
       <c r="A5" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>11</v>
@@ -2283,7 +2276,7 @@
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -2294,7 +2287,7 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="131.25">
       <c r="A6" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>14</v>
@@ -2306,7 +2299,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>16</v>
@@ -2317,7 +2310,7 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="131.25">
       <c r="A7" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>15</v>
@@ -2329,7 +2322,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>17</v>
@@ -2340,49 +2333,49 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="187.5">
       <c r="A8" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>48</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="4"/>
       <c r="E8" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" ht="187.5">
       <c r="A9" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" ht="206.25">
       <c r="A10" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>22</v>
@@ -2394,7 +2387,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>21</v>
@@ -2405,7 +2398,7 @@
     </row>
     <row r="11" spans="1:7" ht="187.5">
       <c r="A11" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>23</v>
@@ -2415,7 +2408,7 @@
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>24</v>
@@ -2426,17 +2419,17 @@
     </row>
     <row r="12" spans="1:7" ht="112.5">
       <c r="A12" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>40</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>27</v>
@@ -2447,195 +2440,195 @@
     </row>
     <row r="13" spans="1:7" ht="56.25">
       <c r="A13" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>44</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="56.25">
       <c r="A14" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="56.25">
       <c r="A15" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>46</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="112.5">
       <c r="A16" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>76</v>
       </c>
       <c r="D16" s="11">
         <v>10</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="150">
       <c r="A17" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D17" s="11"/>
       <c r="E17" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>83</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="131.25">
       <c r="A18" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="D18" s="11"/>
       <c r="E18" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F18" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="10" t="s">
         <v>87</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="168.75">
       <c r="A19" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D19" s="11">
         <v>1</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F19" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>90</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="150">
       <c r="A20" s="12" t="s">
-        <v>47</v>
+        <v>92</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D20" s="11"/>
       <c r="E20" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="93.75">
       <c r="A21" s="12" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="B21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="10" t="s">
         <v>97</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>98</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F21" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="G21" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="G21" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2660,8 +2653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -2676,25 +2669,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="A1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" ht="112.5">
@@ -2709,7 +2702,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>29</v>
@@ -2720,23 +2713,23 @@
     </row>
     <row r="3" spans="1:7" s="1" customFormat="1" ht="56.25">
       <c r="A3" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>94</v>
-      </c>
       <c r="C3" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made the WI pass its own checks.
</commit_message>
<xml_diff>
--- a/Config/JP/Checklist.xlsx
+++ b/Config/JP/Checklist.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64FAA33-C227-4D47-8D0C-7250E9B63141}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07FD6391-1B14-4C11-86B1-69053A346F1F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19410" windowHeight="8865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ワークフロー" sheetId="2" r:id="rId1"/>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="19" spans="1:7" ht="75">
       <c r="A19" s="12" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>

</xml_diff>

<commit_message>
Added Japanese localization of new checks.
</commit_message>
<xml_diff>
--- a/Config/JP/Checklist.xlsx
+++ b/Config/JP/Checklist.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD3227E-E7C3-4CC2-948B-3F1DD42FD953}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{280CDE96-30CD-440D-92EA-84A466315393}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1725,54 +1725,15 @@
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Undocumented Parallel activity</t>
-  </si>
-  <si>
     <t>Checks\Standard\UndocumentedParallelActivity.xaml</t>
-  </si>
-  <si>
-    <t>Using the Parallel activity can make the workflow harder to understand and might lead to unexpected results when combined with UI interactions. If it is necessary to use the Parallel activity, include an annotation to explain the situation.
-For more about the Parallel activity, please refer to https://docs.microsoft.com/en-us/dotnet/api/system.activities.statements.parallel?view=netframework-4.8</t>
-  </si>
-  <si>
-    <t>Verify whether the Parallel activity is really necessary and, if it is, include an annotation explaning why it is being used.</t>
-  </si>
-  <si>
-    <t>Hardcoded password</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Passwords should be stored in secure locations, like Orchestrator or Windows Credential Manager.</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Passwords that are hardcoded into workflows can be a serious security threat since they can be easily recovered by unauthorized parties. For more about protecting sensitive data, please refer to https://docs.uipath.com/studio/docs/protecting-sensitive-information</t>
-    <phoneticPr fontId="5"/>
   </si>
   <si>
     <t>Checks\Standard\HardcodedPassword.xaml</t>
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t>Undocumented Image-based activities</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
     <t>Checks\Standard\UndocumentedImageBasedActivities.xaml</t>
     <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>The use of image-based activities (e.g., Click Image and Wait Image Vanish) is not usually recommended, because they are sensitive to screen resolutions and image quality.
-In cases they must be used, it is a good practice to include an annotation to the activity to explain the situation.</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Confirm whether image-based activities are really necessary and, if they are, add an annotation to explain the situation.</t>
-    <phoneticPr fontId="5"/>
-  </si>
-  <si>
-    <t>Workflow naming convention</t>
-    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>{ 
@@ -1781,31 +1742,11 @@
     <phoneticPr fontId="5"/>
   </si>
   <si>
-    <t xml:space="preserve">Workflows in a project should be named according to the project's naming conventions.  This check receives a regular expression that dictates the naming convention for workflow files. </t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\Custom\WorkflowFileNamingConvention.xaml</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
-    <t>Change the name of the file to match the project's naming conventions.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Mandatory files in project</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
     <t>Checks\Custom\MandatoryFilesInProject.xaml</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>The project should contain mandatory files specified by the COE or project leader. This check receives a list of files that should be in the project folder.</t>
-    <phoneticPr fontId="6"/>
-  </si>
-  <si>
-    <t>Include the mandatory files in the project folder.</t>
     <phoneticPr fontId="6"/>
   </si>
   <si>
@@ -1813,6 +1754,68 @@
   "MandatoryFiles": "Data\\Config.xlsx,Framework\\CloseAllApplications.xaml,Framework\\GetAppCredentials.xaml,Framework\\GetTransactionData.xaml,Framework\\InitAllApplications.xaml,Framework\\InitAllSettings.xaml,Framework\\KillAllProcesses.xaml,Framework\\SetTransactionStatus.xaml,Framework\\TakeScreenshot.xaml,Main.xaml,Process.xaml"
 }</t>
     <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>注釈のないパラレルアクティビティ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>パラレルアクティビティの利用はワークフローの理解しづらくなり、想定外の結果となることがあります。利用が必要な場合は、その理由を説明する注釈を追加してください。パラレルアクティビティについての詳細はこちらを参照ください。
+https://docs.microsoft.com/ja-jp/dotnet/api/system.activities.statements.parallel?view=netframework-4.8</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>パラレルアクティビティの利用が本当に必要か確認してください。必要な場合は、その理由を注釈に記載してください。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>パスワードのハードコーディング</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ハードコードされたパスワードは、想定外の第三者が容易に読み取ることができるためセキュリティ上重大な問題となることがあります。データ保護についての詳細はこちらを参照ください。
+https://docs.uipath.com/studio/lang-ja/docs/protecting-sensitive-information</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>パスワードは、OrchestratorやWindows Credential Manager のようなより安全な場所に格納してください。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>注釈のない画像ベースのアクティビティ</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画像ベースのアクティビティの利用は、挙動の安定性が画素数や画質に依存してしまうため推奨しておりません。利用が必要な場合は、注釈を記載してください。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>画像ベースのアクティビティの利用が本当に必要か確認してください。必要な場合は、理由を説明する注釈を記載してください。</t>
+    <phoneticPr fontId="5"/>
+  </si>
+  <si>
+    <t>ワークフローの命名規則</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ワークフローの命名はプロジェクトで定められた規則に従うべきです。このチェックでは、引数に記載する正規表現によってワークフローの命名規則を定義できます。</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>ワークフローファイル名を命名規則に従うように修正してください。</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>プロジェクトの必須ファイル</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>必ず含まれてなければならない必須ファイルがCoEにより定義されていることがあります。このチェックは、引数で定義された必須ファイルが含まれているかどうか確認します。</t>
+    <phoneticPr fontId="6"/>
+  </si>
+  <si>
+    <t>プロジェクトフォルダに必須ファイルを追加してください。</t>
+    <phoneticPr fontId="6"/>
   </si>
 </sst>
 </file>
@@ -2266,9 +2269,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC94E0F-66AD-4ECB-A9C2-26293DFAAC50}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="18.75"/>
   <cols>
@@ -2671,25 +2672,25 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="13" customFormat="1" ht="168.75">
+    <row r="19" spans="1:7" s="13" customFormat="1" ht="150">
       <c r="A19" s="12" t="s">
         <v>104</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>106</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>107</v>
       </c>
       <c r="D19" s="10"/>
       <c r="E19" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="G19" s="10" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:7" s="13" customFormat="1" ht="112.5">
@@ -2697,41 +2698,41 @@
         <v>104</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G20" s="10" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" ht="131.25">
+    <row r="21" spans="1:7" s="13" customFormat="1" ht="56.25">
       <c r="A21" s="12" t="s">
         <v>104</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D21" s="10"/>
       <c r="E21" s="11" t="s">
         <v>55</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G21" s="10" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="3" customFormat="1" ht="75">
@@ -2739,22 +2740,22 @@
         <v>104</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="E22" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="75">
@@ -2842,9 +2843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCF3B754-2F91-4B5D-866B-FF6D6F8A7738}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
@@ -2926,22 +2925,22 @@
         <v>104</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="E4" s="11" t="s">
         <v>51</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>